<commit_message>
bugs, referral system - done
</commit_message>
<xml_diff>
--- a/accounts_excel_work.xlsx
+++ b/accounts_excel_work.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danila\Desktop\ost_legacy-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\ost_legacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3E4E7A-FE22-4B87-A147-D850FAFB841B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C5E0D4-F478-41A3-8031-0855B76F02C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="705" windowWidth="15810" windowHeight="8820" xr2:uid="{926C0B6E-D700-5743-A140-D345D62463DD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{926C0B6E-D700-5743-A140-D345D62463DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
     <t>birth</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>1192392193239</t>
   </si>
   <si>
@@ -89,6 +86,9 @@
   </si>
   <si>
     <t>CCZN PCTZ JGKB JLJB CHC5 ZZ76 FAF4 Z6ZT</t>
+  </si>
+  <si>
+    <t>DE</t>
   </si>
 </sst>
 </file>
@@ -159,7 +159,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -175,9 +175,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,7 +215,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -321,7 +321,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -474,16 +474,16 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,33 +521,33 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2">
         <v>1685491</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -557,7 +557,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -567,7 +567,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -577,7 +577,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -587,7 +587,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>

</xml_diff>

<commit_message>
changing the account bm, adding varified and types to account and country dbs
</commit_message>
<xml_diff>
--- a/accounts_excel_work.xlsx
+++ b/accounts_excel_work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\ost_legacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D7A12C-0CE9-49F3-A645-F8D284930569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD958464-7BB5-4DEA-ACB3-1E755DE3D0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{926C0B6E-D700-5743-A140-D345D62463DD}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>countryId</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>DE</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>varified</t>
   </si>
 </sst>
 </file>
@@ -468,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DFC89-939D-BD4F-8CC1-1E8995DC5786}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -480,7 +486,7 @@
     <col min="5" max="5" width="11.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,8 +523,11 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -544,17 +553,36 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1192392193239</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1685491</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -564,7 +592,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -574,7 +602,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -584,7 +612,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>

</xml_diff>